<commit_message>
- [`maximizeWindow()`]: FAIL for Electron since it's not supported by underlying driver. - [`goBack()`]: FAIL for Electron since it's not supported by underlying driver.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/data/electron-showcase.data.xlsx
+++ b/src/test/resources/showcase/artifact/data/electron-showcase.data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10610"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76E0DF5-A722-1A4B-B89F-106FC1B85946}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2623564-81A1-924C-AEEF-23981F2ED674}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="15240" windowHeight="9000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>true</t>
   </si>
@@ -97,6 +97,24 @@
   </si>
   <si>
     <t>/Users/ml093043/tools/Electron API Demos.app/Contents/MacOS/Electron API Demos</t>
+  </si>
+  <si>
+    <t>nexial.browser.windowSize</t>
+  </si>
+  <si>
+    <t>maximized</t>
+  </si>
+  <si>
+    <t>nexial.web.alwaysWait</t>
+  </si>
+  <si>
+    <t>nexial.web.highlight</t>
+  </si>
+  <si>
+    <t>nexial.web.highlight.waitMs</t>
+  </si>
+  <si>
+    <t>750</t>
   </si>
 </sst>
 </file>
@@ -580,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AAA10"/>
+  <dimension ref="A1:AAA13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -686,8 +704,38 @@
       <c r="AAA9" s="5"/>
     </row>
     <row r="10" spans="1:703">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="HA10" s="4"/>
       <c r="AAA10" s="5"/>
+    </row>
+    <row r="11" spans="1:703">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:703">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:703">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>

</xml_diff>